<commit_message>
completed some of the supply item system
</commit_message>
<xml_diff>
--- a/Assets/_Excel/skill.xlsx
+++ b/Assets/_Excel/skill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unity\BattleFlagGameStudy\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312D83AE-CF56-4A2E-B2C3-7B8768D1CCD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F218B29A-8050-4CC9-93AC-3D2B3E44AEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="2730" windowWidth="27675" windowHeight="11325" xr2:uid="{2135C274-778A-4362-A271-7BC75D43935F}"/>
+    <workbookView xWindow="645" yWindow="2670" windowWidth="27675" windowHeight="11325" xr2:uid="{2135C274-778A-4362-A271-7BC75D43935F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E499485-6717-4EFD-94E4-80BB7B103708}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1112,13 +1112,13 @@
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1">
         <v>2</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
         <v>1</v>
@@ -1153,13 +1153,13 @@
         <v>5</v>
       </c>
       <c r="E11" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F11" s="1">
         <v>4</v>
       </c>
       <c r="G11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
         <v>1</v>
@@ -1194,13 +1194,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" s="1">
         <v>2</v>
       </c>
       <c r="G12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
         <v>1</v>
@@ -1235,13 +1235,13 @@
         <v>2</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1">
         <v>2</v>
       </c>
       <c r="G13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="1">
         <v>1</v>
@@ -1276,13 +1276,13 @@
         <v>3</v>
       </c>
       <c r="E14" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="1">
         <v>1</v>

</xml_diff>